<commit_message>
[FIX] account_banking_riba: wrong confirmed payment entry
</commit_message>
<xml_diff>
--- a/import_partners/example/example.xlsx
+++ b/import_partners/example/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t xml:space="preserve">Codice</t>
   </si>
@@ -37,13 +37,31 @@
     <t xml:space="preserve">Partita IVA</t>
   </si>
   <si>
-    <t xml:space="preserve">Ref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avere</t>
+    <t xml:space="preserve">Codice fiscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indirizzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Città</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sito web</t>
   </si>
   <si>
     <t xml:space="preserve">Prima Alpha S.p.A.</t>
@@ -52,31 +70,52 @@
     <t xml:space="preserve">IT00115719999</t>
   </si>
   <si>
+    <t xml:space="preserve">Italia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Via I Maggio, 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castano Primo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+39 0255582285</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notaio Decimo Jackson</t>
   </si>
   <si>
     <t xml:space="preserve">IT10242670015</t>
   </si>
   <si>
+    <t xml:space="preserve">JCKLBR72M24L736R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largo Fasuli Decimomanno, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011 2345678</t>
+  </si>
+  <si>
     <t xml:space="preserve">Latte Beta Due s.n.c.</t>
   </si>
   <si>
     <t xml:space="preserve">IT02345670018</t>
   </si>
   <si>
-    <t xml:space="preserve">RiBA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Freie Universität Berlin</t>
   </si>
   <si>
+    <t xml:space="preserve">Germania</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mario Rossi</t>
   </si>
   <si>
     <t xml:space="preserve">RSSMRA69C02D612M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banca</t>
   </si>
 </sst>
 </file>
@@ -151,8 +190,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,153 +212,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1000</v>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>20022</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>250</v>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>10121</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>500</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>152220</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>150</v>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>180003</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>100</v>
-      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>

</xml_diff>